<commit_message>
further ajustments to parameters 3
</commit_message>
<xml_diff>
--- a/excel files/propionate_case_study_v1.xlsx
+++ b/excel files/propionate_case_study_v1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucas\PycharmProjects\Alquimia\excel files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F78BD3FD-FE11-4C60-951A-9F3EDF3251DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C06778C-C036-488D-8BAC-6A306F127D84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="683" xr2:uid="{6BCA81A1-C24E-4458-B51D-F7D92A8A2CBE}"/>
+    <workbookView xWindow="760" yWindow="760" windowWidth="14400" windowHeight="7400" tabRatio="683" activeTab="1" xr2:uid="{6BCA81A1-C24E-4458-B51D-F7D92A8A2CBE}"/>
   </bookViews>
   <sheets>
     <sheet name="input_output_intervals" sheetId="1" r:id="rId1"/>
@@ -4147,7 +4147,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54AE4236-3006-4E07-A9E2-DEE610CD0DBE}">
   <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
@@ -4922,9 +4922,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F85D0432-6958-423D-87F2-E8A979C87816}">
   <dimension ref="A1:W10"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="L1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="P16" sqref="P16"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="M1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="Q10" sqref="Q10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -5567,7 +5567,7 @@
         <v>0</v>
       </c>
       <c r="Q10" s="44">
-        <v>0.64</v>
+        <v>0.77</v>
       </c>
       <c r="R10" s="38" t="s">
         <v>299</v>
@@ -5592,7 +5592,7 @@
   <dimension ref="A1:L10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -5659,7 +5659,7 @@
         <v>60</v>
       </c>
       <c r="D2">
-        <v>0.2</v>
+        <v>0.22</v>
       </c>
       <c r="E2" s="52" t="s">
         <v>61</v>
@@ -5697,7 +5697,7 @@
         <v>60</v>
       </c>
       <c r="D3">
-        <v>0.2</v>
+        <v>0.22</v>
       </c>
       <c r="E3" s="55" t="s">
         <v>61</v>
@@ -5735,7 +5735,7 @@
         <v>60</v>
       </c>
       <c r="D4">
-        <v>0.2</v>
+        <v>0.22</v>
       </c>
       <c r="E4" s="55" t="s">
         <v>61</v>
@@ -5773,7 +5773,7 @@
         <v>60</v>
       </c>
       <c r="D5">
-        <v>0.2</v>
+        <v>0.22</v>
       </c>
       <c r="E5" s="55" t="s">
         <v>61</v>
@@ -5811,7 +5811,7 @@
         <v>60</v>
       </c>
       <c r="D6">
-        <v>0.2</v>
+        <v>0.22</v>
       </c>
       <c r="E6" s="55" t="s">
         <v>61</v>
@@ -5849,7 +5849,7 @@
         <v>60</v>
       </c>
       <c r="D7">
-        <v>0.2</v>
+        <v>0.22</v>
       </c>
       <c r="E7" s="58" t="s">
         <v>61</v>
@@ -5887,7 +5887,7 @@
         <v>60</v>
       </c>
       <c r="D8">
-        <v>0.2</v>
+        <v>0.22</v>
       </c>
       <c r="E8" s="52" t="s">
         <v>61</v>
@@ -5925,7 +5925,7 @@
         <v>60</v>
       </c>
       <c r="D9">
-        <v>0.2</v>
+        <v>0.22</v>
       </c>
       <c r="E9" s="55" t="s">
         <v>61</v>
@@ -5963,7 +5963,7 @@
         <v>60</v>
       </c>
       <c r="D10">
-        <v>0.2</v>
+        <v>0.22</v>
       </c>
       <c r="E10" s="58" t="s">
         <v>61</v>
@@ -6646,7 +6646,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D4 C3 E5 F6 G7 H8">
+  <conditionalFormatting sqref="C3 D4 E5 F6 G7 H8">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>

<commit_message>
adding Metabolic-model of Mixed culture fermetation (matlab)
</commit_message>
<xml_diff>
--- a/excel files/propionate_case_study_v1.xlsx
+++ b/excel files/propionate_case_study_v1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucas\PycharmProjects\Alquimia\excel files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lucas\PycharmProjects\Alquimia\excel files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C06778C-C036-488D-8BAC-6A306F127D84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E27D2956-0BBB-41C4-8D0D-A2F55BFD302C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="760" yWindow="760" windowWidth="14400" windowHeight="7400" tabRatio="683" activeTab="1" xr2:uid="{6BCA81A1-C24E-4458-B51D-F7D92A8A2CBE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="10320" tabRatio="683" activeTab="3" xr2:uid="{6BCA81A1-C24E-4458-B51D-F7D92A8A2CBE}"/>
   </bookViews>
   <sheets>
     <sheet name="input_output_intervals" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="702" uniqueCount="320">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="702" uniqueCount="319">
   <si>
     <t>components</t>
   </si>
@@ -579,9 +579,6 @@
   </si>
   <si>
     <t xml:space="preserve">seperation efficientcy </t>
-  </si>
-  <si>
-    <t>TOFIND (see DWA?)</t>
   </si>
   <si>
     <t>https://doi.org/10.1186/s13068-019-1433-7</t>
@@ -1586,7 +1583,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
@@ -3849,9 +3846,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - Tema de 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -3889,7 +3886,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -3995,7 +3992,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -4137,7 +4134,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -4151,7 +4148,7 @@
       <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="5.453125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
@@ -4203,7 +4200,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C2" s="4">
         <v>1000</v>
@@ -4212,10 +4209,10 @@
         <v>1000</v>
       </c>
       <c r="E2" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="F2" s="32" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="G2" s="4">
         <v>0</v>
@@ -4224,7 +4221,7 @@
         <v>60</v>
       </c>
       <c r="I2" s="32" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="J2" s="4">
         <v>1</v>
@@ -4244,7 +4241,7 @@
         <v>27</v>
       </c>
       <c r="E3" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="F3" s="4">
         <v>0</v>
@@ -4276,7 +4273,7 @@
         <v>27</v>
       </c>
       <c r="E4" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="F4" s="4">
         <v>0</v>
@@ -4319,7 +4316,7 @@
       <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="17.54296875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.7265625" bestFit="1" customWidth="1"/>
@@ -4331,13 +4328,13 @@
         <v>85</v>
       </c>
       <c r="B1" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C1" t="s">
         <v>59</v>
       </c>
       <c r="D1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E1" t="s">
         <v>119</v>
@@ -4348,13 +4345,13 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="25" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B2">
         <v>0.37</v>
       </c>
       <c r="C2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D2" s="69">
         <f>B2*1/1.1</f>
@@ -4364,18 +4361,18 @@
         <v>60</v>
       </c>
       <c r="F2" s="36" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="77" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B3">
         <v>1.85</v>
       </c>
       <c r="C3" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D3" s="69">
         <f t="shared" ref="D3:D12" si="0">B3*1/1.1</f>
@@ -4385,18 +4382,18 @@
         <v>60</v>
       </c>
       <c r="F3" s="36" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="25" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B4">
         <v>0.4</v>
       </c>
       <c r="C4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D4" s="69">
         <f t="shared" si="0"/>
@@ -4406,18 +4403,18 @@
         <v>60</v>
       </c>
       <c r="F4" s="36" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="25" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B5">
         <v>0.51</v>
       </c>
       <c r="C5" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D5" s="69">
         <f t="shared" si="0"/>
@@ -4427,18 +4424,18 @@
         <v>60</v>
       </c>
       <c r="F5" s="36" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="25" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B6">
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D6" s="69">
         <f t="shared" si="0"/>
@@ -4448,18 +4445,18 @@
         <v>60</v>
       </c>
       <c r="F6" s="36" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="77" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B7">
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D7" s="69">
         <f t="shared" si="0"/>
@@ -4469,18 +4466,18 @@
         <v>60</v>
       </c>
       <c r="F7" s="36" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="25" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B8">
         <v>3.5</v>
       </c>
       <c r="C8" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D8" s="69">
         <f t="shared" si="0"/>
@@ -4490,18 +4487,18 @@
         <v>60</v>
       </c>
       <c r="F8" s="36" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="25" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B9">
         <v>0.85</v>
       </c>
       <c r="C9" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D9" s="69">
         <f t="shared" si="0"/>
@@ -4511,18 +4508,18 @@
         <v>60</v>
       </c>
       <c r="F9" s="36" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="25" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B10">
         <v>0.45</v>
       </c>
       <c r="C10" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D10" s="69">
         <f t="shared" si="0"/>
@@ -4532,19 +4529,19 @@
         <v>60</v>
       </c>
       <c r="F10" s="36" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="45" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B11">
         <f>2.25 *1.1</f>
         <v>2.4750000000000001</v>
       </c>
       <c r="C11" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D11" s="69">
         <f t="shared" si="0"/>
@@ -4554,19 +4551,19 @@
         <v>60</v>
       </c>
       <c r="F11" s="36" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="45" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B12">
         <f>1.165</f>
         <v>1.165</v>
       </c>
       <c r="C12" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D12" s="69">
         <f t="shared" si="0"/>
@@ -4576,7 +4573,7 @@
         <v>60</v>
       </c>
       <c r="F12" s="36" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -4613,7 +4610,7 @@
       <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="17.54296875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="55.1796875" bestFit="1" customWidth="1"/>
@@ -4624,7 +4621,7 @@
         <v>85</v>
       </c>
       <c r="B1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C1" t="s">
         <v>59</v>
@@ -4635,7 +4632,7 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="25" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B2">
         <v>222</v>
@@ -4644,12 +4641,12 @@
         <v>60</v>
       </c>
       <c r="D2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="25" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B3">
         <v>85.8</v>
@@ -4658,12 +4655,12 @@
         <v>60</v>
       </c>
       <c r="D3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="25" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B4">
         <v>64.3</v>
@@ -4672,12 +4669,12 @@
         <v>60</v>
       </c>
       <c r="D4" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="25" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B5">
         <v>74.8</v>
@@ -4686,12 +4683,12 @@
         <v>60</v>
       </c>
       <c r="D5" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="25" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B6">
         <v>61.1</v>
@@ -4700,12 +4697,12 @@
         <v>60</v>
       </c>
       <c r="D6" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="25" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B7">
         <v>381</v>
@@ -4714,12 +4711,12 @@
         <v>60</v>
       </c>
       <c r="D7" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="25" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B8">
         <v>53.6</v>
@@ -4728,12 +4725,12 @@
         <v>60</v>
       </c>
       <c r="D8" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="25" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B9">
         <v>53.3</v>
@@ -4742,12 +4739,12 @@
         <v>60</v>
       </c>
       <c r="D9" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="25" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B10">
         <v>52.3</v>
@@ -4756,12 +4753,12 @@
         <v>60</v>
       </c>
       <c r="D10" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="25" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B11">
         <v>78.5</v>
@@ -4770,15 +4767,15 @@
         <v>60</v>
       </c>
       <c r="D11" s="36" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E11" s="37" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="25" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B12">
         <v>50.5</v>
@@ -4787,10 +4784,10 @@
         <v>60</v>
       </c>
       <c r="D12" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E12" s="37" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -4810,7 +4807,7 @@
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="11.453125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.90625" bestFit="1" customWidth="1"/>
@@ -4820,27 +4817,27 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
+        <v>203</v>
+      </c>
+      <c r="B1" t="s">
         <v>204</v>
-      </c>
-      <c r="B1" t="s">
-        <v>205</v>
       </c>
       <c r="C1" t="s">
         <v>59</v>
       </c>
       <c r="D1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="E1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="4" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B2" s="4">
         <v>37</v>
@@ -4849,21 +4846,21 @@
         <v>67</v>
       </c>
       <c r="D2" s="36" t="s">
+        <v>211</v>
+      </c>
+      <c r="E2" s="43" t="s">
         <v>212</v>
       </c>
-      <c r="E2" s="43" t="s">
-        <v>213</v>
-      </c>
       <c r="F2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="4" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C3" t="s">
         <v>67</v>
@@ -4871,31 +4868,31 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="4" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="4" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="4" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="4" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B7" s="4">
         <v>71</v>
@@ -4904,10 +4901,10 @@
         <v>67</v>
       </c>
       <c r="D7" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F7" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
   </sheetData>
@@ -4922,12 +4919,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F85D0432-6958-423D-87F2-E8A979C87816}">
   <dimension ref="A1:W10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="M1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="Q10" sqref="Q10"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="P1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="S9" sqref="S9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="17.26953125" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="17.26953125" customWidth="1"/>
@@ -4979,7 +4976,7 @@
         <v>66</v>
       </c>
       <c r="I1" s="41" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="J1" s="41" t="s">
         <v>108</v>
@@ -5026,7 +5023,7 @@
         <v>116</v>
       </c>
       <c r="D2" s="39" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E2" s="38" t="s">
         <v>72</v>
@@ -5050,7 +5047,7 @@
         <v>0</v>
       </c>
       <c r="L2" s="38" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="M2" s="38" t="s">
         <v>99</v>
@@ -5059,7 +5056,7 @@
         <v>72</v>
       </c>
       <c r="O2" s="65" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="P2" s="38">
         <v>0</v>
@@ -5069,7 +5066,7 @@
         <v>5.0000000000000001E-4</v>
       </c>
       <c r="R2" s="38" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="V2">
         <v>0</v>
@@ -5089,7 +5086,7 @@
         <v>116</v>
       </c>
       <c r="D3" s="39" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E3" s="38" t="s">
         <v>72</v>
@@ -5113,7 +5110,7 @@
         <v>0</v>
       </c>
       <c r="L3" s="38" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="M3" s="38" t="s">
         <v>99</v>
@@ -5122,7 +5119,7 @@
         <v>72</v>
       </c>
       <c r="O3" s="65" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="P3" s="38">
         <v>0</v>
@@ -5132,7 +5129,7 @@
         <v>5.0000000000000001E-4</v>
       </c>
       <c r="R3" s="38" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="V3">
         <v>0</v>
@@ -5152,7 +5149,7 @@
         <v>116</v>
       </c>
       <c r="D4" s="39" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E4" s="38" t="s">
         <v>72</v>
@@ -5176,7 +5173,7 @@
         <v>0</v>
       </c>
       <c r="L4" s="38" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="M4" s="38" t="s">
         <v>99</v>
@@ -5185,7 +5182,7 @@
         <v>72</v>
       </c>
       <c r="O4" s="65" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="P4" s="38">
         <v>0</v>
@@ -5195,7 +5192,7 @@
         <v>5.0000000000000001E-4</v>
       </c>
       <c r="R4" s="38" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="V4">
         <v>0</v>
@@ -5215,7 +5212,7 @@
         <v>116</v>
       </c>
       <c r="D5" s="39" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E5" s="38" t="s">
         <v>72</v>
@@ -5239,7 +5236,7 @@
         <v>0</v>
       </c>
       <c r="L5" s="38" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="M5" s="38" t="s">
         <v>99</v>
@@ -5248,7 +5245,7 @@
         <v>72</v>
       </c>
       <c r="O5" s="65" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="P5" s="38">
         <v>0</v>
@@ -5258,7 +5255,7 @@
         <v>5.0000000000000001E-4</v>
       </c>
       <c r="R5" s="38" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="V5">
         <v>0</v>
@@ -5278,7 +5275,7 @@
         <v>116</v>
       </c>
       <c r="D6" s="39" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E6" s="38" t="s">
         <v>72</v>
@@ -5302,7 +5299,7 @@
         <v>0</v>
       </c>
       <c r="L6" s="38" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="M6" s="38" t="s">
         <v>99</v>
@@ -5311,7 +5308,7 @@
         <v>72</v>
       </c>
       <c r="O6" s="65" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="P6" s="38">
         <v>0</v>
@@ -5321,7 +5318,7 @@
         <v>5.0000000000000001E-4</v>
       </c>
       <c r="R6" s="38" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="V6">
         <v>0</v>
@@ -5341,7 +5338,7 @@
         <v>116</v>
       </c>
       <c r="D7" s="39" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E7" s="38" t="s">
         <v>72</v>
@@ -5374,7 +5371,7 @@
         <v>72</v>
       </c>
       <c r="O7" s="65" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="P7" s="38">
         <v>0</v>
@@ -5384,7 +5381,7 @@
         <v>5.0000000000000001E-4</v>
       </c>
       <c r="R7" s="38" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="V7">
         <v>0</v>
@@ -5419,7 +5416,7 @@
         <v>4.473795180722892E-4</v>
       </c>
       <c r="I8" s="38" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="J8" s="38">
         <v>0</v>
@@ -5437,7 +5434,7 @@
         <v>72</v>
       </c>
       <c r="O8" s="66" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="P8" s="38">
         <v>0</v>
@@ -5446,7 +5443,7 @@
         <v>0.113</v>
       </c>
       <c r="R8" s="38" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="V8">
         <v>0</v>
@@ -5499,7 +5496,7 @@
         <v>72</v>
       </c>
       <c r="O9" s="67" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="P9" s="38">
         <v>0</v>
@@ -5508,7 +5505,7 @@
         <v>0.27</v>
       </c>
       <c r="R9" s="38" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="V9" t="s">
         <v>79</v>
@@ -5561,7 +5558,7 @@
         <v>72</v>
       </c>
       <c r="O10" s="67" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="P10" s="38">
         <v>0</v>
@@ -5570,7 +5567,7 @@
         <v>0.77</v>
       </c>
       <c r="R10" s="38" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="V10">
         <v>0</v>
@@ -5595,7 +5592,7 @@
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="17.36328125" customWidth="1"/>
     <col min="2" max="2" width="13.26953125" bestFit="1" customWidth="1"/>
@@ -5683,7 +5680,7 @@
         <v>64</v>
       </c>
       <c r="L2" s="75" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -5721,7 +5718,7 @@
         <v>64</v>
       </c>
       <c r="L3" s="75" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -5759,7 +5756,7 @@
         <v>64</v>
       </c>
       <c r="L4" s="75" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="5" spans="1:12">
@@ -5797,7 +5794,7 @@
         <v>64</v>
       </c>
       <c r="L5" s="75" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -5835,7 +5832,7 @@
         <v>64</v>
       </c>
       <c r="L6" s="75" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="7" spans="1:12">
@@ -5873,7 +5870,7 @@
         <v>64</v>
       </c>
       <c r="L7" s="75" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="8" spans="1:12">
@@ -5911,7 +5908,7 @@
         <v>64</v>
       </c>
       <c r="L8" s="75" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -5949,7 +5946,7 @@
         <v>64</v>
       </c>
       <c r="L9" s="75" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -5987,7 +5984,7 @@
         <v>64</v>
       </c>
       <c r="L10" s="75" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
   </sheetData>
@@ -6001,12 +5998,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6BC952C-F64C-4F30-9DDA-924F82AF01AE}">
   <dimension ref="A1:N14"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="16.54296875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.453125" bestFit="1" customWidth="1"/>
@@ -6024,7 +6021,7 @@
         <v>6</v>
       </c>
       <c r="B1" s="17" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C1" s="28" t="s">
         <v>103</v>
@@ -6065,7 +6062,7 @@
     </row>
     <row r="2" spans="1:14">
       <c r="A2" s="29" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B2" s="12">
         <v>0</v>
@@ -6444,7 +6441,7 @@
         <v>0</v>
       </c>
       <c r="J10" s="5" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="K10" s="6" t="s">
         <v>23</v>
@@ -6646,7 +6643,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C3 D4 E5 F6 G7 H8">
+  <conditionalFormatting sqref="D4 C3 E5 F6 G7 H8">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -6671,7 +6668,7 @@
       <selection pane="topRight" activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.90625" defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="43.08984375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.6328125" bestFit="1" customWidth="1"/>
@@ -6689,7 +6686,7 @@
         <v>29</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>30</v>
@@ -6715,10 +6712,10 @@
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="38" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B2" s="27" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C2" s="27">
         <v>0</v>
@@ -6744,10 +6741,10 @@
     </row>
     <row r="3" spans="1:9">
       <c r="A3" s="38" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B3" s="27" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C3" s="27">
         <v>0</v>
@@ -6773,10 +6770,10 @@
     </row>
     <row r="4" spans="1:9">
       <c r="A4" s="38" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B4" s="27" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C4" s="27">
         <v>0</v>
@@ -6802,10 +6799,10 @@
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="38" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B5" s="27" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C5" s="27">
         <v>0</v>
@@ -6831,10 +6828,10 @@
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="38" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B6" s="27" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C6" s="27">
         <v>0</v>
@@ -6872,10 +6869,10 @@
         <v>46</v>
       </c>
       <c r="E7" s="33" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F7" s="33" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="G7" s="34">
         <v>0</v>
@@ -6915,7 +6912,7 @@
       <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="11.81640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.81640625" bestFit="1" customWidth="1"/>
@@ -7120,7 +7117,7 @@
       <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.90625" defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="11.453125" bestFit="1" customWidth="1"/>
   </cols>
@@ -7239,10 +7236,10 @@
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B15" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
   </sheetData>
@@ -7258,7 +7255,7 @@
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
   <cols>
     <col min="2" max="2" width="25.453125" bestFit="1" customWidth="1"/>
   </cols>
@@ -7404,11 +7401,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE819A9C-4E64-4D0F-8F31-2F1BF4DCFD79}">
   <dimension ref="A1:AA36"/>
   <sheetViews>
-    <sheetView topLeftCell="T1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Y20" sqref="Y20"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="29.1796875" customWidth="1"/>
     <col min="2" max="4" width="37.7265625" bestFit="1" customWidth="1"/>
@@ -7437,10 +7434,10 @@
     </row>
     <row r="2" spans="1:27">
       <c r="P2" s="68" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="X2" s="68" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="3" spans="1:27">
@@ -7451,7 +7448,7 @@
         <v>170</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>71</v>
@@ -7470,25 +7467,25 @@
       </c>
       <c r="J3" s="4"/>
       <c r="K3" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="M3" s="1" t="s">
         <v>237</v>
       </c>
-      <c r="L3" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>238</v>
-      </c>
       <c r="N3" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="Q3" s="1" t="s">
         <v>234</v>
       </c>
-      <c r="P3" s="1" t="s">
-        <v>257</v>
-      </c>
-      <c r="Q3" s="1" t="s">
-        <v>235</v>
-      </c>
       <c r="R3" s="1" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="S3" s="1" t="s">
         <v>57</v>
@@ -7498,8 +7495,8 @@
       <c r="A4" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="20" t="s">
-        <v>171</v>
+      <c r="B4" s="4" t="s">
+        <v>159</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>167</v>
@@ -7514,52 +7511,52 @@
         <v>167</v>
       </c>
       <c r="H4" s="72" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="I4" s="50" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="K4">
         <v>30</v>
       </c>
       <c r="L4" t="s">
+        <v>239</v>
+      </c>
+      <c r="M4" t="s">
+        <v>238</v>
+      </c>
+      <c r="N4" t="s">
         <v>240</v>
-      </c>
-      <c r="M4" t="s">
-        <v>239</v>
-      </c>
-      <c r="N4" t="s">
-        <v>241</v>
       </c>
       <c r="P4">
         <v>0.129</v>
       </c>
       <c r="Q4" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="R4" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="S4" s="36" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="X4" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="Y4" s="56">
         <f>(0.5 +0.17 +0.38+0.08) *1000</f>
         <v>1130.0000000000002</v>
       </c>
       <c r="Z4" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="5" spans="1:27">
       <c r="A5" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="20" t="s">
-        <v>171</v>
+      <c r="B5" s="4" t="s">
+        <v>159</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>167</v>
@@ -7574,37 +7571,37 @@
         <v>167</v>
       </c>
       <c r="H5" s="72" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="I5" s="50" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="K5">
         <v>52.5</v>
       </c>
       <c r="L5" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="M5" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="N5" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="P5">
         <v>0.127</v>
       </c>
       <c r="Q5" t="s">
+        <v>251</v>
+      </c>
+      <c r="R5" t="s">
+        <v>250</v>
+      </c>
+      <c r="S5" s="36" t="s">
         <v>252</v>
       </c>
-      <c r="R5" t="s">
-        <v>251</v>
-      </c>
-      <c r="S5" s="36" t="s">
-        <v>253</v>
-      </c>
       <c r="X5" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="Y5">
         <v>9960</v>
@@ -7617,8 +7614,8 @@
       <c r="A6" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="20" t="s">
-        <v>171</v>
+      <c r="B6" s="4" t="s">
+        <v>159</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>167</v>
@@ -7633,25 +7630,25 @@
         <v>167</v>
       </c>
       <c r="H6" s="72" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="I6" s="50" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="K6">
         <v>44.62</v>
       </c>
       <c r="L6" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="M6" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="N6" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="X6" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="Y6">
         <v>11363</v>
@@ -7664,8 +7661,8 @@
       <c r="A7" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="20" t="s">
-        <v>171</v>
+      <c r="B7" s="4" t="s">
+        <v>159</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>167</v>
@@ -7680,18 +7677,18 @@
         <v>167</v>
       </c>
       <c r="H7" s="72" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="I7" s="50" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="8" spans="1:27" ht="15" thickBot="1">
       <c r="A8" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="B8" s="20" t="s">
-        <v>171</v>
+      <c r="B8" s="4" t="s">
+        <v>159</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>167</v>
@@ -7706,44 +7703,44 @@
         <v>167</v>
       </c>
       <c r="H8" s="72" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="I8" s="50" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="K8" s="47" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="L8" s="48">
         <f>AVERAGE(K4:K6)</f>
         <v>42.373333333333335</v>
       </c>
       <c r="M8" s="49" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="P8" s="68" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="R8" s="36" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="X8" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="Y8" s="70">
         <f xml:space="preserve"> Y4/(Y5 )</f>
         <v>0.1134538152610442</v>
       </c>
       <c r="Z8" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="9" spans="1:27">
       <c r="A9" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="B9" s="20" t="s">
-        <v>171</v>
+      <c r="B9" s="4" t="s">
+        <v>159</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>167</v>
@@ -7758,22 +7755,22 @@
         <v>167</v>
       </c>
       <c r="H9" s="72" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="I9" s="50" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="P9" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="Q9" s="1" t="s">
         <v>258</v>
       </c>
-      <c r="Q9" s="1" t="s">
-        <v>259</v>
-      </c>
       <c r="R9" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="X9" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="10" spans="1:27">
@@ -7781,7 +7778,7 @@
         <v>53</v>
       </c>
       <c r="B10" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C10" t="s">
         <v>168</v>
@@ -7793,39 +7790,39 @@
         <v>167</v>
       </c>
       <c r="G10" s="20" t="s">
+        <v>274</v>
+      </c>
+      <c r="H10" s="72" t="s">
         <v>275</v>
       </c>
-      <c r="H10" s="72" t="s">
+      <c r="I10" s="73" t="s">
         <v>276</v>
       </c>
-      <c r="I10" s="73" t="s">
-        <v>277</v>
-      </c>
       <c r="P10" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="Q10">
         <v>400</v>
       </c>
       <c r="R10" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="X10" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="11" spans="1:27">
       <c r="A11" s="15" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>167</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="E11" s="4" t="s">
         <v>167</v>
@@ -7834,19 +7831,19 @@
         <v>167</v>
       </c>
       <c r="H11" s="72" t="s">
+        <v>275</v>
+      </c>
+      <c r="I11" s="73" t="s">
         <v>276</v>
       </c>
-      <c r="I11" s="73" t="s">
-        <v>277</v>
-      </c>
       <c r="P11" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="Q11" s="69">
         <v>2.83</v>
       </c>
       <c r="R11" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="12" spans="1:27">
@@ -7854,7 +7851,7 @@
         <v>50</v>
       </c>
       <c r="B12" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>167</v>
@@ -7869,22 +7866,22 @@
         <v>167</v>
       </c>
       <c r="H12" s="72" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="I12" s="73" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="P12" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="Q12">
         <v>0.38</v>
       </c>
       <c r="R12" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="X12" s="68" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="13" spans="1:27">
@@ -7892,7 +7889,7 @@
         <v>51</v>
       </c>
       <c r="B13" s="26" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>167</v>
@@ -7907,28 +7904,28 @@
         <v>167</v>
       </c>
       <c r="H13" s="72" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="I13" s="73" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="P13" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="Q13">
         <v>30</v>
       </c>
       <c r="R13" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="X13" s="1" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="Y13" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="Z13" s="1" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="AA13" s="1" t="s">
         <v>57</v>
@@ -7939,7 +7936,7 @@
         <v>52</v>
       </c>
       <c r="B14" s="26" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>167</v>
@@ -7954,13 +7951,13 @@
         <v>167</v>
       </c>
       <c r="H14" s="72" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="I14" s="73" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="X14" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="Y14">
         <v>9960</v>
@@ -7972,14 +7969,14 @@
     <row r="15" spans="1:27">
       <c r="C15" s="4"/>
       <c r="P15" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="Q15" s="69">
         <f>Q11*Q12*Q13</f>
         <v>32.262</v>
       </c>
       <c r="R15" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="X15" t="s">
         <v>93</v>
@@ -7988,7 +7985,7 @@
         <v>9902</v>
       </c>
       <c r="Z15" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="AA15" s="36" t="s">
         <v>168</v>
@@ -7997,14 +7994,14 @@
     <row r="16" spans="1:27">
       <c r="C16" s="4"/>
       <c r="P16" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="Q16">
         <f>Q15/Q10</f>
         <v>8.0655000000000004E-2</v>
       </c>
       <c r="X16" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="Y16">
         <v>0.45</v>
@@ -8013,7 +8010,7 @@
         <v>67</v>
       </c>
       <c r="AA16" s="36" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="17" spans="16:26">
@@ -8022,17 +8019,17 @@
         <v>8.0655000000000001</v>
       </c>
       <c r="R17" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="X17" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="Y17">
         <f xml:space="preserve"> Y15*Y16</f>
         <v>4455.9000000000005</v>
       </c>
       <c r="Z17" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="18" spans="16:26">
@@ -8046,101 +8043,101 @@
     </row>
     <row r="20" spans="16:26">
       <c r="X20" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="Y20" s="56">
         <f>Y18/Y14</f>
         <v>4.473795180722892E-4</v>
       </c>
       <c r="Z20" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="26" spans="16:26">
       <c r="P26" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="Q26">
         <v>400</v>
       </c>
       <c r="R26" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="27" spans="16:26">
       <c r="P27" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="Q27">
         <f>Q26/3600</f>
         <v>0.1111111111111111</v>
       </c>
       <c r="R27" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="29" spans="16:26">
       <c r="P29" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="Q29">
         <v>20</v>
       </c>
       <c r="R29" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="30" spans="16:26">
       <c r="P30" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="Q30">
         <f>Q29 *100</f>
         <v>2000</v>
       </c>
       <c r="R30" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="32" spans="16:26">
       <c r="P32" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="Q32">
         <f>Q30*Q27</f>
         <v>222.2222222222222</v>
       </c>
       <c r="R32" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="33" spans="16:18">
       <c r="P33" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="Q33">
         <f>Q32</f>
         <v>222.2222222222222</v>
       </c>
       <c r="R33" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="35" spans="16:18">
       <c r="P35" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="Q35">
         <f>Q33/Q26</f>
         <v>0.55555555555555547</v>
       </c>
       <c r="R35" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="36" spans="16:18">
       <c r="P36" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
   </sheetData>

</xml_diff>